<commit_message>
Successful Effort excel creation
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10155"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -43,6 +38,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,000"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -64,12 +62,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6F738"/>
+        <bgColor rgb="FFE6F738"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -119,19 +123,116 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="SAPMemberCell" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -157,15 +258,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -180,39 +273,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +337,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +371,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -291,151 +382,175 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -444,55 +559,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A11">
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>